<commit_message>
Final - Main Spreadsheet w/out chats
</commit_message>
<xml_diff>
--- a/Final_Capstone_Spreadsheet.xlsx
+++ b/Final_Capstone_Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2A9E13-400E-4776-AFEC-1B30C8935AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7AF656-2234-46CD-AC67-12318D4D60AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C84C568-BB1D-4E22-BFF7-82713F13B653}"/>
+    <workbookView xWindow="2250" yWindow="1050" windowWidth="20550" windowHeight="14550" xr2:uid="{5C84C568-BB1D-4E22-BFF7-82713F13B653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -311,6 +311,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -627,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332728E2-40ED-4FF8-A63E-ACB59181D2D0}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,6 +1994,12 @@
         <v>16458</v>
       </c>
     </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F22" s="7">
+        <f>SUM(F2:F21)</f>
+        <v>3373650000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>